<commit_message>
PRI176: Update Daypart parser to support TTNW and CNN daypart formats
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/CNNAMPMBarterObligations_AllBadDayparts.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/CNNAMPMBarterObligations_AllBadDayparts.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\Broadcast\OnDeck\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oleksandr\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Active AM &amp; PM Barter" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -102,10 +102,10 @@
     <t>ENCT</t>
   </si>
   <si>
-    <t>10-10:30P:M-F</t>
-  </si>
-  <si>
     <t>5:30:A-6A:M-F                           8A-9A:M-FL</t>
+  </si>
+  <si>
+    <t>10??10:30P:M-F</t>
   </si>
 </sst>
 </file>
@@ -480,14 +480,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="41">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 3 2" xfId="23"/>
     <cellStyle name="Comma 4" xfId="24"/>
     <cellStyle name="Currency 2" xfId="2"/>
     <cellStyle name="Currency 2 2" xfId="3"/>
     <cellStyle name="Currency 3" xfId="4"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="6"/>
     <cellStyle name="Normal 2 2" xfId="7"/>
     <cellStyle name="Normal 2 3" xfId="8"/>
@@ -521,6 +518,9 @@
     <cellStyle name="Normal 2 6" xfId="15"/>
     <cellStyle name="Normal 2 6 2" xfId="33"/>
     <cellStyle name="Normal 2 7" xfId="25"/>
+    <cellStyle name="Гиперссылка" xfId="5" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -536,9 +536,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -576,7 +576,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -611,23 +611,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -663,26 +646,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -858,7 +824,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -945,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="71" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J2" s="72">
         <v>42887</v>
@@ -986,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3" s="49">
         <v>42842</v>

</xml_diff>